<commit_message>
update - working on purrr/functions
</commit_message>
<xml_diff>
--- a/part5/data/patient_example.xlsx
+++ b/part5/data/patient_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\ready_for_r_labs\part5\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\sph_r_programming\part5\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271867A4-9423-4958-99C9-0CB894A0F6A5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16B001A-57D0-4B79-B559-8E1A31D9A504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{82F6687A-6AAC-4D82-AE23-6AA6B3C1DC39}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{82F6687A-6AAC-4D82-AE23-6AA6B3C1DC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>first_name</t>
   </si>
@@ -67,6 +62,9 @@
   </si>
   <si>
     <t>patient_id</t>
+  </si>
+  <si>
+    <t>date_of_birth</t>
   </si>
 </sst>
 </file>
@@ -102,8 +100,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,21 +417,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231B9BAA-016D-401C-84B8-BBE6EA651635}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -445,8 +445,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2333</v>
       </c>
@@ -459,8 +462,11 @@
       <c r="D2">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" s="1">
+        <v>16755</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>7359</v>
       </c>
@@ -473,8 +479,11 @@
       <c r="D3">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" s="1">
+        <v>33197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1414</v>
       </c>
@@ -487,8 +496,11 @@
       <c r="D4">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4" s="1">
+        <v>28247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>8424</v>
       </c>
@@ -500,6 +512,9 @@
       </c>
       <c r="D5">
         <v>14</v>
+      </c>
+      <c r="E5" s="1">
+        <v>38756</v>
       </c>
     </row>
   </sheetData>
@@ -513,9 +528,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -523,7 +538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2333</v>
       </c>
@@ -531,7 +546,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>7359</v>
       </c>
@@ -539,7 +554,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1414</v>
       </c>
@@ -547,7 +562,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4409</v>
       </c>

</xml_diff>